<commit_message>
Add analysis to find how many projects each student signed up for
</commit_message>
<xml_diff>
--- a/signups.xlsx
+++ b/signups.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W2</t>
   </si>
   <si>
     <t xml:space="preserve">X2</t>
@@ -321,10 +324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1174,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1194,7 +1197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1294,9 +1297,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="n">
         <v>1</v>
@@ -1314,9 +1317,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="n">
         <v>1</v>
@@ -1334,9 +1337,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B52" s="2" t="n">
         <v>1</v>
@@ -1354,9 +1357,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B53" s="2" t="n">
         <v>1</v>
@@ -1374,9 +1377,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B54" s="2" t="n">
         <v>0</v>
@@ -1394,9 +1397,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B55" s="2" t="n">
         <v>0</v>
@@ -1414,9 +1417,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B56" s="2" t="n">
         <v>0</v>
@@ -1434,9 +1437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="n">
         <v>0</v>
@@ -1454,6 +1457,9 @@
         <v>0</v>
       </c>
     </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>